<commit_message>
updating CHNOSZ and NMDS
</commit_message>
<xml_diff>
--- a/MineralReactions/DeMMO_mineralRxns.xlsx
+++ b/MineralReactions/DeMMO_mineralRxns.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Caitlin/Desktop/DeMMO_BiofilmPub2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Caitlin/Desktop/DeMMO_BiofilmPub2018/DeMMO_BiofilmPub2019/MineralReactions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5ABAE7C7-7A09-2843-A43E-999DD11813C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10918221-E026-824A-93C4-17789E9D4ABC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{B49AA465-D857-0243-A3F9-EF2FE9DCD461}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15920" xr2:uid="{B49AA465-D857-0243-A3F9-EF2FE9DCD461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="59">
   <si>
     <t>rxn.number</t>
   </si>
@@ -159,9 +164,6 @@
     <t>NO2-</t>
   </si>
   <si>
-    <t>CH4</t>
-  </si>
-  <si>
     <t>HCO3-</t>
   </si>
   <si>
@@ -199,6 +201,12 @@
   </si>
   <si>
     <t>pyrite</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>methane</t>
   </si>
 </sst>
 </file>
@@ -625,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F47464-C3AB-1F4D-A4C3-B5851BA84376}">
-  <dimension ref="A1:AE34"/>
+  <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="AE29" sqref="AE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -778,7 +786,7 @@
         <v>36</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>38</v>
@@ -934,13 +942,13 @@
         <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>33</v>
@@ -949,7 +957,7 @@
         <v>34</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>35</v>
@@ -979,7 +987,7 @@
         <v>36</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y5" s="3" t="s">
         <v>38</v>
@@ -1002,13 +1010,13 @@
         <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>35</v>
@@ -1017,7 +1025,7 @@
         <v>34</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>33</v>
@@ -1085,7 +1093,7 @@
         <v>34</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>35</v>
@@ -1138,13 +1146,13 @@
         <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>33</v>
@@ -1153,7 +1161,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>35</v>
@@ -1198,91 +1206,85 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:31" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="5" t="s">
+    <row r="9" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="5">
-        <v>2</v>
-      </c>
-      <c r="N9" s="5">
-        <v>-1</v>
-      </c>
-      <c r="O9" s="5">
-        <v>-1</v>
-      </c>
-      <c r="P9" s="5">
-        <v>-6</v>
-      </c>
-      <c r="R9" s="5">
-        <v>3</v>
-      </c>
-      <c r="S9" s="5">
-        <v>4</v>
+      <c r="H9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9" s="3">
+        <v>2</v>
+      </c>
+      <c r="N9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="O9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="P9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="R9" s="3">
+        <v>1</v>
+      </c>
+      <c r="S9" s="3">
+        <v>1</v>
       </c>
       <c r="W9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="X9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y9" s="5" t="s">
+      <c r="X9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="AA9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AB9" s="5" t="s">
-        <v>39</v>
+      <c r="AB9" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:31" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M10" s="5">
@@ -1295,15 +1297,12 @@
         <v>-1</v>
       </c>
       <c r="P10" s="5">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="R10" s="5">
         <v>3</v>
       </c>
       <c r="S10" s="5">
-        <v>1</v>
-      </c>
-      <c r="T10" s="5">
         <v>4</v>
       </c>
       <c r="W10" s="3" t="s">
@@ -1319,60 +1318,57 @@
         <v>38</v>
       </c>
       <c r="AB10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC10" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:31" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M11" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N11" s="5">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="O11" s="5">
         <v>-1</v>
       </c>
       <c r="P11" s="5">
-        <v>-16</v>
+        <v>-7</v>
       </c>
       <c r="R11" s="5">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="S11" s="5">
         <v>1</v>
       </c>
       <c r="T11" s="5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="W11" s="3" t="s">
         <v>36</v>
@@ -1387,7 +1383,7 @@
         <v>38</v>
       </c>
       <c r="AB11" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AC11" s="5" t="s">
         <v>39</v>
@@ -1395,58 +1391,58 @@
     </row>
     <row r="12" spans="1:31" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M12" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N12" s="5">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="O12" s="5">
         <v>-1</v>
       </c>
       <c r="P12" s="5">
-        <v>-23</v>
+        <v>-16</v>
       </c>
       <c r="R12" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="S12" s="5">
         <v>1</v>
       </c>
       <c r="T12" s="5">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="W12" s="3" t="s">
         <v>36</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>38</v>
@@ -1463,58 +1459,58 @@
     </row>
     <row r="13" spans="1:31" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M13" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N13" s="5">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="O13" s="5">
         <v>-1</v>
       </c>
       <c r="P13" s="5">
-        <v>-16</v>
+        <v>-23</v>
       </c>
       <c r="R13" s="5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="S13" s="5">
         <v>1</v>
       </c>
       <c r="T13" s="5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="W13" s="3" t="s">
         <v>36</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Y13" s="5" t="s">
         <v>38</v>
@@ -1531,58 +1527,58 @@
     </row>
     <row r="14" spans="1:31" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M14" s="5">
+        <v>6</v>
+      </c>
+      <c r="N14" s="5">
+        <v>-3</v>
+      </c>
+      <c r="O14" s="5">
+        <v>-1</v>
+      </c>
+      <c r="P14" s="5">
+        <v>-16</v>
+      </c>
+      <c r="R14" s="5">
+        <v>9</v>
+      </c>
+      <c r="S14" s="5">
+        <v>1</v>
+      </c>
+      <c r="T14" s="5">
         <v>8</v>
       </c>
-      <c r="N14" s="5">
-        <v>-4</v>
-      </c>
-      <c r="O14" s="5">
-        <v>-1</v>
-      </c>
-      <c r="P14" s="5">
-        <v>-23</v>
-      </c>
-      <c r="R14" s="5">
-        <v>12</v>
-      </c>
-      <c r="S14" s="5">
-        <v>2</v>
-      </c>
-      <c r="T14" s="5">
-        <v>12</v>
-      </c>
       <c r="W14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="X14" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Y14" s="5" t="s">
         <v>38</v>
@@ -1598,254 +1594,246 @@
       </c>
     </row>
     <row r="15" spans="1:31" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
-        <v>14</v>
+      <c r="A15" s="5">
+        <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="M15" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N15" s="5">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="O15" s="5">
+        <v>-1</v>
+      </c>
+      <c r="P15" s="5">
+        <v>-23</v>
+      </c>
+      <c r="R15" s="5">
+        <v>12</v>
+      </c>
+      <c r="S15" s="5">
+        <v>2</v>
+      </c>
+      <c r="T15" s="5">
+        <v>12</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC15" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" s="5">
+        <v>2</v>
+      </c>
+      <c r="N16" s="5">
+        <v>-1</v>
+      </c>
+      <c r="O16" s="5">
         <v>-2</v>
       </c>
-      <c r="P15" s="5">
+      <c r="P16" s="5">
         <v>-2</v>
       </c>
-      <c r="R15" s="5">
+      <c r="R16" s="5">
         <v>3</v>
       </c>
-      <c r="S15" s="5">
-        <v>2</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB15" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="S16" s="5">
+        <v>2</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB16" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" s="8">
-        <v>8</v>
-      </c>
-      <c r="N16" s="8">
-        <v>-1</v>
-      </c>
-      <c r="O16" s="8">
-        <v>-4</v>
-      </c>
-      <c r="P16" s="8">
-        <v>-1</v>
-      </c>
-      <c r="R16" s="8">
-        <v>1</v>
-      </c>
-      <c r="S16" s="8">
-        <v>1</v>
-      </c>
-      <c r="T16" s="8">
-        <v>6</v>
-      </c>
-      <c r="W16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC16" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
-        <v>16</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M17" s="8">
-        <v>8</v>
-      </c>
-      <c r="N17" s="8">
-        <v>-1</v>
-      </c>
-      <c r="O17" s="8">
-        <v>-3</v>
-      </c>
-      <c r="P17" s="8">
+      <c r="H17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="5">
+        <v>2</v>
+      </c>
+      <c r="N17" s="5">
+        <v>-1</v>
+      </c>
+      <c r="O17" s="5">
+        <v>-1</v>
+      </c>
+      <c r="P17" s="5">
         <v>-5</v>
       </c>
-      <c r="R17" s="8">
-        <v>1</v>
-      </c>
-      <c r="S17" s="8">
-        <v>1</v>
-      </c>
-      <c r="T17" s="8">
-        <v>6</v>
+      <c r="R17" s="5">
+        <v>3</v>
+      </c>
+      <c r="S17" s="5">
+        <v>1</v>
+      </c>
+      <c r="T17" s="5">
+        <v>2</v>
       </c>
       <c r="W17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="X17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA17" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC17" s="8" t="s">
+      <c r="X17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC17" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>42</v>
+        <v>32</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>40</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M18" s="8">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="N18" s="8">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="O18" s="8">
         <v>-4</v>
       </c>
+      <c r="P18" s="8">
+        <v>-1</v>
+      </c>
       <c r="R18" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S18" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T18" s="8">
-        <v>3</v>
-      </c>
-      <c r="U18" s="8">
-        <v>10</v>
-      </c>
-      <c r="V18" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W18" s="3" t="s">
         <v>36</v>
@@ -1853,48 +1841,45 @@
       <c r="X18" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AA18" s="8" t="s">
+      <c r="Y18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA18" s="3" t="s">
         <v>38</v>
       </c>
       <c r="AB18" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AC18" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD18" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE18" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="J19" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K19" s="8" t="s">
         <v>35</v>
       </c>
       <c r="M19" s="8">
@@ -1904,7 +1889,10 @@
         <v>-1</v>
       </c>
       <c r="O19" s="8">
-        <v>-1</v>
+        <v>-3</v>
+      </c>
+      <c r="P19" s="8">
+        <v>-5</v>
       </c>
       <c r="R19" s="8">
         <v>1</v>
@@ -1913,84 +1901,81 @@
         <v>1</v>
       </c>
       <c r="T19" s="8">
-        <v>1</v>
-      </c>
-      <c r="U19" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="W19" s="3" t="s">
         <v>36</v>
       </c>
       <c r="X19" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="AA19" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AB19" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AC19" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD19" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>40</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="8" t="s">
         <v>33</v>
       </c>
       <c r="M20" s="8">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="N20" s="8">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="O20" s="8">
-        <v>-8</v>
-      </c>
-      <c r="P20" s="8">
-        <v>-10</v>
+        <v>-4</v>
       </c>
       <c r="R20" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S20" s="8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="T20" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U20" s="8">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="V20" s="8">
+        <v>5</v>
       </c>
       <c r="W20" s="3" t="s">
         <v>36</v>
@@ -1998,82 +1983,76 @@
       <c r="X20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Y20" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="AA20" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AB20" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AC20" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AD20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE20" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>40</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="L21" s="8" t="s">
         <v>35</v>
       </c>
       <c r="M21" s="8">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="N21" s="8">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="O21" s="8">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="R21" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S21" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T21" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U21" s="8">
         <v>3</v>
       </c>
-      <c r="V21" s="8">
-        <v>2</v>
-      </c>
       <c r="W21" s="3" t="s">
         <v>36</v>
       </c>
       <c r="X21" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AA21" s="8" t="s">
         <v>38</v>
@@ -2085,39 +2064,39 @@
         <v>38</v>
       </c>
       <c r="AD21" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE21" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>40</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M22" s="8">
         <v>8</v>
@@ -2126,19 +2105,22 @@
         <v>-1</v>
       </c>
       <c r="O22" s="8">
-        <v>-1</v>
+        <v>-8</v>
+      </c>
+      <c r="P22" s="8">
+        <v>-10</v>
       </c>
       <c r="R22" s="8">
         <v>1</v>
       </c>
       <c r="S22" s="8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="T22" s="8">
         <v>1</v>
       </c>
       <c r="U22" s="8">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="W22" s="3" t="s">
         <v>36</v>
@@ -2146,567 +2128,595 @@
       <c r="X22" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="Y22" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="AA22" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AB22" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AC22" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AD22" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
+      <c r="A23" s="8">
+        <v>20</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M23" s="8">
+        <v>24</v>
+      </c>
+      <c r="N23" s="8">
+        <v>-3</v>
+      </c>
+      <c r="O23" s="8">
+        <v>-4</v>
+      </c>
+      <c r="R23" s="8">
+        <v>4</v>
+      </c>
+      <c r="S23" s="8">
+        <v>3</v>
+      </c>
+      <c r="T23" s="8">
+        <v>5</v>
+      </c>
+      <c r="U23" s="8">
+        <v>3</v>
+      </c>
+      <c r="V23" s="8">
+        <v>2</v>
+      </c>
+      <c r="W23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE23" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>21</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M24" s="8">
+        <v>8</v>
+      </c>
+      <c r="N24" s="8">
+        <v>-1</v>
+      </c>
+      <c r="O24" s="8">
+        <v>-1</v>
+      </c>
+      <c r="R24" s="8">
+        <v>1</v>
+      </c>
+      <c r="S24" s="8">
+        <v>2</v>
+      </c>
+      <c r="T24" s="8">
+        <v>1</v>
+      </c>
+      <c r="U24" s="8">
+        <v>2</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD24" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="K25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="8">
+        <v>8</v>
+      </c>
+      <c r="N25" s="8">
+        <v>-1</v>
+      </c>
+      <c r="O25" s="8">
+        <v>-8</v>
+      </c>
+      <c r="P25" s="8">
+        <v>-10</v>
+      </c>
+      <c r="R25" s="8">
+        <v>1</v>
+      </c>
+      <c r="S25" s="8">
+        <v>8</v>
+      </c>
+      <c r="T25" s="8">
+        <v>1</v>
+      </c>
+      <c r="U25" s="8">
+        <v>15</v>
+      </c>
+      <c r="W25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD25" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" s="8" t="s">
+      <c r="J26" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M26" s="8">
+        <v>8</v>
+      </c>
+      <c r="N26" s="8">
+        <v>-1</v>
+      </c>
+      <c r="O26" s="8">
+        <v>-4</v>
+      </c>
+      <c r="P26" s="8">
+        <v>-2</v>
+      </c>
+      <c r="R26" s="8">
+        <v>1</v>
+      </c>
+      <c r="S26" s="8">
+        <v>1</v>
+      </c>
+      <c r="T26" s="8">
+        <v>4</v>
+      </c>
+      <c r="U26" s="8">
+        <v>3</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X26" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA26" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB26" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC26" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD26" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>23</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="10">
+        <v>2</v>
+      </c>
+      <c r="N27" s="10">
+        <v>-2</v>
+      </c>
+      <c r="O27" s="10">
+        <v>-1</v>
+      </c>
+      <c r="P27" s="10">
+        <v>-3</v>
+      </c>
+      <c r="R27" s="10">
+        <v>2</v>
+      </c>
+      <c r="S27" s="10">
+        <v>1</v>
+      </c>
+      <c r="T27" s="10">
+        <v>2</v>
+      </c>
+      <c r="U27" s="10">
+        <v>2</v>
+      </c>
+      <c r="W27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD27" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="10">
+        <v>24</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K23" s="8" t="s">
+      <c r="J28" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K28" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="M23" s="8">
+      <c r="M28" s="10">
         <v>8</v>
       </c>
-      <c r="N23" s="8">
-        <v>-1</v>
-      </c>
-      <c r="O23" s="8">
+      <c r="N28" s="10">
         <v>-8</v>
       </c>
-      <c r="P23" s="8">
-        <v>-10</v>
-      </c>
-      <c r="R23" s="8">
-        <v>1</v>
-      </c>
-      <c r="S23" s="8">
+      <c r="O28" s="10">
+        <v>-1</v>
+      </c>
+      <c r="P28" s="10">
+        <v>-12</v>
+      </c>
+      <c r="R28" s="10">
         <v>8</v>
       </c>
-      <c r="T23" s="8">
-        <v>1</v>
-      </c>
-      <c r="U23" s="8">
-        <v>15</v>
-      </c>
-      <c r="W23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB23" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD23" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10">
-        <v>23</v>
-      </c>
-      <c r="B24" s="10" t="s">
+      <c r="S28" s="10">
+        <v>1</v>
+      </c>
+      <c r="T28" s="10">
+        <v>8</v>
+      </c>
+      <c r="U28" s="10">
+        <v>7</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y28" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA28" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD28" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="10" t="s">
+      <c r="D29" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K24" s="10" t="s">
+      <c r="E29" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K29" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="M24" s="10">
-        <v>2</v>
-      </c>
-      <c r="N24" s="10">
-        <v>-2</v>
-      </c>
-      <c r="O24" s="10">
-        <v>-1</v>
-      </c>
-      <c r="P24" s="10">
-        <v>-3</v>
-      </c>
-      <c r="R24" s="10">
-        <v>2</v>
-      </c>
-      <c r="S24" s="10">
-        <v>1</v>
-      </c>
-      <c r="T24" s="10">
-        <v>2</v>
-      </c>
-      <c r="U24" s="10">
-        <v>2</v>
-      </c>
-      <c r="W24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X24" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y24" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA24" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB24" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC24" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD24" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10">
-        <v>24</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="M25" s="10">
-        <v>8</v>
-      </c>
-      <c r="N25" s="10">
-        <v>-8</v>
-      </c>
-      <c r="O25" s="10">
-        <v>-1</v>
-      </c>
-      <c r="P25" s="10">
-        <v>-12</v>
-      </c>
-      <c r="R25" s="10">
-        <v>8</v>
-      </c>
-      <c r="S25" s="10">
-        <v>1</v>
-      </c>
-      <c r="T25" s="10">
-        <v>8</v>
-      </c>
-      <c r="U25" s="10">
-        <v>7</v>
-      </c>
-      <c r="W25" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X25" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y25" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA25" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB25" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC25" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD25" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12">
-        <v>25</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M26" s="12">
-        <v>2</v>
-      </c>
-      <c r="N26" s="12">
-        <v>-1</v>
-      </c>
-      <c r="O26" s="12">
-        <v>-1</v>
-      </c>
-      <c r="P26" s="12">
-        <v>-4</v>
-      </c>
-      <c r="R26" s="12">
-        <v>2</v>
-      </c>
-      <c r="S26" s="12">
-        <v>3</v>
-      </c>
-      <c r="W26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X26" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y26" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA26" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB26" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12">
-        <v>26</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M27" s="12">
-        <v>2</v>
-      </c>
-      <c r="N27" s="12">
-        <v>-1</v>
-      </c>
-      <c r="O27" s="12">
-        <v>-1</v>
-      </c>
-      <c r="P27" s="12">
-        <v>-5</v>
-      </c>
-      <c r="R27" s="12">
-        <v>2</v>
-      </c>
-      <c r="S27" s="12">
-        <v>1</v>
-      </c>
-      <c r="T27" s="12">
-        <v>3</v>
-      </c>
-      <c r="W27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X27" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y27" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA27" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB27" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC27" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12">
-        <v>27</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M28" s="12">
+      <c r="M29" s="10">
         <v>6</v>
       </c>
-      <c r="N28" s="12">
-        <v>-3</v>
-      </c>
-      <c r="O28" s="12">
-        <v>-1</v>
-      </c>
-      <c r="P28" s="12">
-        <v>-10</v>
-      </c>
-      <c r="R28" s="12">
+      <c r="N29" s="10">
+        <v>-6</v>
+      </c>
+      <c r="O29" s="10">
+        <v>-1</v>
+      </c>
+      <c r="P29" s="10">
+        <v>-11</v>
+      </c>
+      <c r="R29" s="10">
         <v>6</v>
       </c>
-      <c r="S28" s="12">
-        <v>1</v>
-      </c>
-      <c r="T28" s="12">
-        <v>7</v>
-      </c>
-      <c r="W28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X28" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y28" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA28" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB28" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC28" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12">
-        <v>28</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M29" s="12">
-        <v>8</v>
-      </c>
-      <c r="N29" s="12">
-        <v>-4</v>
-      </c>
-      <c r="O29" s="12">
-        <v>-1</v>
-      </c>
-      <c r="P29" s="12">
-        <v>-15</v>
-      </c>
-      <c r="R29" s="12">
-        <v>8</v>
-      </c>
-      <c r="S29" s="12">
-        <v>1</v>
-      </c>
-      <c r="T29" s="12">
-        <v>9</v>
+      <c r="S29" s="10">
+        <v>6</v>
+      </c>
+      <c r="T29" s="10">
+        <v>1</v>
+      </c>
+      <c r="U29" s="10">
+        <v>6</v>
       </c>
       <c r="W29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="X29" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y29" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA29" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB29" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC29" s="12" t="s">
-        <v>39</v>
+      <c r="X29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y29" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD29" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J30" s="12" t="s">
         <v>35</v>
       </c>
       <c r="M30" s="12">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N30" s="12">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="O30" s="12">
         <v>-1</v>
       </c>
       <c r="P30" s="12">
-        <v>-10</v>
+        <v>-4</v>
       </c>
       <c r="R30" s="12">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S30" s="12">
-        <v>1</v>
-      </c>
-      <c r="T30" s="12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W30" s="3" t="s">
         <v>36</v>
       </c>
       <c r="X30" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Y30" s="12" t="s">
         <v>38</v>
@@ -2715,273 +2725,673 @@
         <v>38</v>
       </c>
       <c r="AB30" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC30" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I31" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M31" s="12">
+        <v>2</v>
+      </c>
+      <c r="N31" s="12">
+        <v>-1</v>
+      </c>
+      <c r="O31" s="12">
+        <v>-1</v>
+      </c>
+      <c r="P31" s="12">
+        <v>-5</v>
+      </c>
+      <c r="R31" s="12">
+        <v>2</v>
+      </c>
+      <c r="S31" s="12">
+        <v>1</v>
+      </c>
+      <c r="T31" s="12">
+        <v>3</v>
+      </c>
+      <c r="W31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB31" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC31" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12">
+        <v>27</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="J31" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M31" s="12">
+      <c r="I32" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M32" s="12">
+        <v>6</v>
+      </c>
+      <c r="N32" s="12">
+        <v>-3</v>
+      </c>
+      <c r="O32" s="12">
+        <v>-1</v>
+      </c>
+      <c r="P32" s="12">
+        <v>-10</v>
+      </c>
+      <c r="R32" s="12">
+        <v>6</v>
+      </c>
+      <c r="S32" s="12">
+        <v>1</v>
+      </c>
+      <c r="T32" s="12">
+        <v>7</v>
+      </c>
+      <c r="W32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC32" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="12">
+        <v>28</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M33" s="12">
         <v>8</v>
       </c>
-      <c r="N31" s="12">
+      <c r="N33" s="12">
         <v>-4</v>
       </c>
-      <c r="O31" s="12">
-        <v>-1</v>
-      </c>
-      <c r="P31" s="12">
+      <c r="O33" s="12">
+        <v>-1</v>
+      </c>
+      <c r="P33" s="12">
         <v>-15</v>
       </c>
-      <c r="R31" s="12">
+      <c r="R33" s="12">
         <v>8</v>
       </c>
-      <c r="S31" s="12">
-        <v>2</v>
-      </c>
-      <c r="T31" s="12">
+      <c r="S33" s="12">
+        <v>1</v>
+      </c>
+      <c r="T33" s="12">
+        <v>9</v>
+      </c>
+      <c r="W33" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC33" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12">
+        <v>29</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M34" s="12">
+        <v>6</v>
+      </c>
+      <c r="N34" s="12">
+        <v>-3</v>
+      </c>
+      <c r="O34" s="12">
+        <v>-1</v>
+      </c>
+      <c r="P34" s="12">
+        <v>-10</v>
+      </c>
+      <c r="R34" s="12">
+        <v>6</v>
+      </c>
+      <c r="S34" s="12">
+        <v>1</v>
+      </c>
+      <c r="T34" s="12">
+        <v>5</v>
+      </c>
+      <c r="W34" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X34" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y34" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA34" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB34" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC34" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12">
+        <v>30</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M35" s="12">
         <v>8</v>
       </c>
-      <c r="W31" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X31" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y31" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA31" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB31" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC31" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
+      <c r="N35" s="12">
+        <v>-4</v>
+      </c>
+      <c r="O35" s="12">
+        <v>-1</v>
+      </c>
+      <c r="P35" s="12">
+        <v>-15</v>
+      </c>
+      <c r="R35" s="12">
+        <v>8</v>
+      </c>
+      <c r="S35" s="12">
+        <v>2</v>
+      </c>
+      <c r="T35" s="12">
+        <v>8</v>
+      </c>
+      <c r="W35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC35" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B36" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M36" s="12">
+        <v>2</v>
+      </c>
+      <c r="N36" s="12">
+        <v>-1</v>
+      </c>
+      <c r="O36" s="12">
+        <v>-2</v>
+      </c>
+      <c r="P36" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R36" s="12">
+        <v>2</v>
+      </c>
+      <c r="S36" s="12">
+        <v>2</v>
+      </c>
+      <c r="W36" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X36" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y36" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA36" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB36" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M37" s="12">
+        <v>2</v>
+      </c>
+      <c r="N37" s="12">
+        <v>-1</v>
+      </c>
+      <c r="O37" s="12">
+        <v>-1</v>
+      </c>
+      <c r="P37" s="12">
+        <v>-3</v>
+      </c>
+      <c r="R37" s="12">
+        <v>2</v>
+      </c>
+      <c r="S37" s="12">
+        <v>1</v>
+      </c>
+      <c r="T37" s="12">
+        <v>1</v>
+      </c>
+      <c r="W37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC37" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="14">
+        <v>32</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="13" t="s">
+      <c r="D38" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="M32" s="12">
-        <v>2</v>
-      </c>
-      <c r="N32" s="12">
-        <v>-1</v>
-      </c>
-      <c r="O32" s="12">
+      <c r="E38" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M38" s="14">
+        <v>16</v>
+      </c>
+      <c r="N38" s="14">
+        <v>-1</v>
+      </c>
+      <c r="O38" s="14">
+        <v>-8</v>
+      </c>
+      <c r="R38" s="14">
+        <v>1</v>
+      </c>
+      <c r="S38" s="14">
+        <v>2</v>
+      </c>
+      <c r="T38" s="14">
+        <v>8</v>
+      </c>
+      <c r="W38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X38" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA38" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB38" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC38" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="14">
+        <v>33</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="M39" s="14">
+        <v>16</v>
+      </c>
+      <c r="N39" s="14">
+        <v>-1</v>
+      </c>
+      <c r="O39" s="14">
         <v>-2</v>
       </c>
-      <c r="P32" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R32" s="12">
-        <v>2</v>
-      </c>
-      <c r="S32" s="12">
-        <v>2</v>
-      </c>
-      <c r="W32" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X32" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y32" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA32" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB32" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="14">
-        <v>32</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="14" t="s">
+      <c r="P39" s="14">
+        <v>-2</v>
+      </c>
+      <c r="Q39" s="14">
+        <v>-2</v>
+      </c>
+      <c r="R39" s="14">
+        <v>1</v>
+      </c>
+      <c r="S39" s="14">
+        <v>2</v>
+      </c>
+      <c r="T39" s="14">
+        <v>2</v>
+      </c>
+      <c r="W39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X39" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y39" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z39" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA39" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB39" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC39" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="C40" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I33" s="14" t="s">
+      <c r="F40" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="M40" s="14">
         <v>48</v>
       </c>
-      <c r="J33" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="M33" s="14">
-        <v>16</v>
-      </c>
-      <c r="N33" s="14">
-        <v>-1</v>
-      </c>
-      <c r="O33" s="14">
+      <c r="N40" s="14">
+        <v>-3</v>
+      </c>
+      <c r="O40" s="14">
         <v>-8</v>
       </c>
-      <c r="R33" s="14">
-        <v>1</v>
-      </c>
-      <c r="S33" s="14">
-        <v>2</v>
-      </c>
-      <c r="T33" s="14">
+      <c r="P40" s="14">
+        <v>-16</v>
+      </c>
+      <c r="R40" s="14">
+        <v>3</v>
+      </c>
+      <c r="S40" s="14">
+        <v>6</v>
+      </c>
+      <c r="T40" s="14">
         <v>8</v>
       </c>
-      <c r="W33" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X33" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA33" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB33" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC33" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="14">
-        <v>33</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="J34" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="M34" s="14">
-        <v>16</v>
-      </c>
-      <c r="N34" s="14">
-        <v>-1</v>
-      </c>
-      <c r="O34" s="14">
-        <v>-2</v>
-      </c>
-      <c r="P34" s="14">
-        <v>-2</v>
-      </c>
-      <c r="Q34" s="14">
-        <v>-2</v>
-      </c>
-      <c r="R34" s="14">
-        <v>1</v>
-      </c>
-      <c r="S34" s="14">
-        <v>2</v>
-      </c>
-      <c r="T34" s="14">
-        <v>2</v>
-      </c>
-      <c r="W34" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X34" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y34" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z34" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA34" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB34" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC34" s="14" t="s">
-        <v>37</v>
+      <c r="W40" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X40" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y40" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA40" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB40" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC40" s="14" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>